<commit_message>
Logic harness слюнигер support
</commit_message>
<xml_diff>
--- a/Control Box 12V.xlsx
+++ b/Control Box 12V.xlsx
@@ -16,244 +16,244 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="80">
   <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>DC/DC 12V Vout+</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>70442-SD-100</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>70806-SD-100</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>G09</t>
+  </si>
+  <si>
+    <t>14 FERRULE</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>TXL 14</t>
+  </si>
+  <si>
+    <t>Wire Item</t>
+  </si>
+  <si>
+    <t>70802-SD-100</t>
+  </si>
+  <si>
+    <t>TXL 20</t>
+  </si>
+  <si>
+    <t>Vout1-</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Vout2-</t>
+  </si>
+  <si>
+    <t>11+</t>
+  </si>
+  <si>
+    <t>12V BUS A Disable</t>
+  </si>
+  <si>
+    <t>18 FERRULE</t>
+  </si>
+  <si>
+    <t>PS12</t>
+  </si>
+  <si>
+    <t>Vout1+</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>PS5</t>
+  </si>
+  <si>
+    <t>DC/DC 12V Vout-</t>
+  </si>
+  <si>
+    <t>20 FERRULE</t>
+  </si>
+  <si>
+    <t>70991-SD-100</t>
+  </si>
+  <si>
+    <t>TXL 18</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>70992-SD-100</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>G20</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>70804-SD-100</t>
   </si>
   <si>
-    <t>-</t>
+    <t>27.5</t>
+  </si>
+  <si>
+    <t>70494-SD-100</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>Vin+</t>
+  </si>
+  <si>
+    <t>Vout2+</t>
+  </si>
+  <si>
+    <t>12 FERRULE</t>
+  </si>
+  <si>
+    <t>Termination</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>Drive Lights</t>
+  </si>
+  <si>
+    <t>Device</t>
   </si>
   <si>
     <t>G02</t>
   </si>
   <si>
-    <t>K2</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>70806-SD-100</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>70442-SD-100</t>
-  </si>
-  <si>
-    <t>27.5</t>
-  </si>
-  <si>
-    <t>Vout1-</t>
-  </si>
-  <si>
-    <t>TXL 14</t>
+    <t>DC/DC 5V Vin-</t>
+  </si>
+  <si>
+    <t>Steering Brake</t>
+  </si>
+  <si>
+    <t>182a</t>
+  </si>
+  <si>
+    <t>DC/DC 5V Vin+</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>182b</t>
+  </si>
+  <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>F12A4</t>
   </si>
   <si>
     <t>70807-SD-100</t>
   </si>
   <si>
-    <t>14 FERRULE</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>DC/DC 12V Vout+</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>PS12</t>
-  </si>
-  <si>
-    <t>F12A4</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12V BUS A Disable</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>183</t>
-  </si>
-  <si>
-    <t>Drive Lights</t>
-  </si>
-  <si>
-    <t>18 FERRULE</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>70440-SD-100</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>F12A3</t>
+  </si>
+  <si>
+    <t>70493-SD-100</t>
+  </si>
+  <si>
+    <t>33</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>PS5</t>
-  </si>
-  <si>
-    <t>70440-SD-100</t>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Vin-</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Pin</t>
   </si>
   <si>
     <t>F12A5</t>
   </si>
   <si>
-    <t>20 FERRULE</t>
-  </si>
-  <si>
-    <t>181</t>
+    <t>SSR1</t>
+  </si>
+  <si>
+    <t>12V BUA A Enable</t>
   </si>
   <si>
     <t>^</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Wire</t>
-  </si>
-  <si>
-    <t>Pin</t>
-  </si>
-  <si>
-    <t>Vout1+</t>
-  </si>
-  <si>
-    <t>G09</t>
-  </si>
-  <si>
-    <t>70991-SD-100</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>F12A3</t>
-  </si>
-  <si>
-    <t>12V BUA A Enable</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>70992-SD-100</t>
-  </si>
-  <si>
-    <t>TXL 18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>70493-SD-100</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>Vout2-</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>SSR1</t>
-  </si>
-  <si>
-    <t>K3</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>TXL 20</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>182a</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>70802-SD-100</t>
-  </si>
-  <si>
-    <t>70494-SD-100</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>12 FERRULE</t>
-  </si>
-  <si>
-    <t>182b</t>
-  </si>
-  <si>
-    <t>Vout2+</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>Wire Item</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>DC/DC 12V Vout-</t>
-  </si>
-  <si>
-    <t>Termination</t>
-  </si>
-  <si>
-    <t>DC/DC 5V Vin+</t>
-  </si>
-  <si>
-    <t>Vin+</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>DC/DC 5V Vin-</t>
-  </si>
-  <si>
-    <t>11+</t>
-  </si>
-  <si>
-    <t>Steering Brake</t>
-  </si>
-  <si>
-    <t>Vin-</t>
-  </si>
-  <si>
-    <t>G20</t>
-  </si>
-  <si>
-    <t>33</t>
   </si>
 </sst>
 </file>
@@ -865,84 +865,84 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="4" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>29</v>
@@ -954,313 +954,313 @@
         <v>1</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="13" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>32</v>
       </c>
       <c r="K3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="16" t="s">
-        <v>5</v>
-      </c>
       <c r="M3" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="22" t="s">
+      <c r="K4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>37</v>
-      </c>
       <c r="O4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>38</v>
-      </c>
       <c r="I5" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>32</v>
       </c>
       <c r="K5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>5</v>
-      </c>
       <c r="M5" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="O5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F6" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>14</v>
-      </c>
       <c r="K6" s="29" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="M6" s="28"/>
       <c r="N6" s="27" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="O6" s="28" t="s">
         <v>1</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="13" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>13</v>
-      </c>
       <c r="F7" s="16" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>32</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>1</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O8" s="16" t="s">
         <v>1</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>3</v>
@@ -1269,140 +1269,140 @@
         <v>1</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L9" s="28" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="M9" s="28" t="s">
         <v>29</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="O9" s="28" t="s">
         <v>1</v>
       </c>
       <c r="P9" s="30" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="30" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="N10" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="O10" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="30" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="33" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>32</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="L11" s="34" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N11" s="33" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="O11" s="34" t="s">
         <v>1</v>
       </c>
       <c r="P11" s="36" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>